<commit_message>
Scaffolded coontrollers and views of Degreeplan and student.
</commit_message>
<xml_diff>
--- a/Docs/DatabaseSamples.xlsx
+++ b/Docs/DatabaseSamples.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531367\Documents\44663\Team01Repo\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\masters\C#.net\MSACSDegreePlan\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812808C8-BEEF-4BFF-AE81-195C8DC8F69F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="Student" sheetId="6" r:id="rId6"/>
     <sheet name="StudentTerm" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="76">
   <si>
     <t>ACS+2</t>
   </si>
@@ -149,12 +148,6 @@
     <t>summer off</t>
   </si>
   <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>Last</t>
-  </si>
-  <si>
     <t>Snumber</t>
   </si>
   <si>
@@ -252,12 +245,30 @@
   </si>
   <si>
     <t>new Requirement{</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>_919number</t>
+  </si>
+  <si>
+    <t>DegreePlanAbrev</t>
+  </si>
+  <si>
+    <t>DegreePlanName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -326,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -334,10 +345,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -618,10 +637,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -654,7 +673,7 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="str">
+      <c r="D2" s="7" t="str">
         <f>C2&amp;$A$1&amp;"="&amp;A2&amp;","</f>
         <v>MS ACS +2 DegreeID=1,</v>
       </c>
@@ -666,10 +685,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -686,10 +705,10 @@
         <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -703,14 +722,14 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F2" t="str">
         <f>$E$2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;"'"&amp;B2&amp;"'"&amp;","&amp;$C$1&amp;"="&amp;"'"&amp;C2&amp;"'"&amp;$G$2</f>
         <v>new Requirement{RequirementID=460,RequirementAbbrev='DB',RequirementName='44-460 Database'}</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -899,7 +918,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -915,7 +934,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
         <v>31</v>
@@ -1139,10 +1158,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1151,24 +1170,24 @@
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" customWidth="1"/>
-    <col min="5" max="5" width="85.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="85.7109375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
         <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>67</v>
+      <c r="E1" s="8" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1184,7 +1203,7 @@
       <c r="D2">
         <v>460</v>
       </c>
-      <c r="E2" s="9" t="str">
+      <c r="E2" s="8" t="str">
         <f>"new DegreePlanTermRequirement{"&amp;$A$1&amp;"="&amp;A2&amp;$B$1&amp;"="&amp;B2&amp;$C$1&amp;"="&amp;C2&amp;$D$1&amp;"="&amp;D2</f>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=1DegreePlanID=10TermID=1RequirementID=460</v>
       </c>
@@ -1202,7 +1221,7 @@
       <c r="D3">
         <v>356</v>
       </c>
-      <c r="E3" s="9" t="str">
+      <c r="E3" s="8" t="str">
         <f>"new DegreePlanTermRequirement{"&amp;$A$1&amp;"="&amp;A3&amp;$B$1&amp;"="&amp;B3&amp;$C$1&amp;"="&amp;C3&amp;$D$1&amp;"="&amp;D3</f>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=2DegreePlanID=10TermID=1RequirementID=356</v>
       </c>
@@ -1220,7 +1239,7 @@
       <c r="D4">
         <v>542</v>
       </c>
-      <c r="E4" s="9" t="str">
+      <c r="E4" s="8" t="str">
         <f t="shared" ref="E4:E66" si="0">"new DegreePlanTermRequirement{"&amp;$A$1&amp;"="&amp;A4&amp;$B$1&amp;"="&amp;B4&amp;$C$1&amp;"="&amp;C4&amp;$D$1&amp;"="&amp;D4</f>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=3DegreePlanID=10TermID=1RequirementID=542</v>
       </c>
@@ -1238,7 +1257,7 @@
       <c r="D5">
         <v>563</v>
       </c>
-      <c r="E5" s="9" t="str">
+      <c r="E5" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=4DegreePlanID=10TermID=1RequirementID=563</v>
       </c>
@@ -1256,7 +1275,7 @@
       <c r="D6">
         <v>560</v>
       </c>
-      <c r="E6" s="9" t="str">
+      <c r="E6" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=5DegreePlanID=10TermID=2RequirementID=560</v>
       </c>
@@ -1274,7 +1293,7 @@
       <c r="D7">
         <v>555</v>
       </c>
-      <c r="E7" s="9" t="str">
+      <c r="E7" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=6DegreePlanID=10TermID=2RequirementID=555</v>
       </c>
@@ -1292,7 +1311,7 @@
       <c r="D8">
         <v>618</v>
       </c>
-      <c r="E8" s="9" t="str">
+      <c r="E8" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=7DegreePlanID=10TermID=2RequirementID=618</v>
       </c>
@@ -1310,7 +1329,7 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" s="9" t="str">
+      <c r="E9" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=8DegreePlanID=10TermID=3RequirementID=1</v>
       </c>
@@ -1328,7 +1347,7 @@
       <c r="D10">
         <v>664</v>
       </c>
-      <c r="E10" s="9" t="str">
+      <c r="E10" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=9DegreePlanID=10TermID=3RequirementID=664</v>
       </c>
@@ -1346,7 +1365,7 @@
       <c r="D11">
         <v>691</v>
       </c>
-      <c r="E11" s="9" t="str">
+      <c r="E11" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=10DegreePlanID=10TermID=3RequirementID=691</v>
       </c>
@@ -1364,7 +1383,7 @@
       <c r="D12">
         <v>10</v>
       </c>
-      <c r="E12" s="9" t="str">
+      <c r="E12" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=11DegreePlanID=10TermID=4RequirementID=10</v>
       </c>
@@ -1382,7 +1401,7 @@
       <c r="D13">
         <v>20</v>
       </c>
-      <c r="E13" s="9" t="str">
+      <c r="E13" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=12DegreePlanID=10TermID=4RequirementID=20</v>
       </c>
@@ -1400,7 +1419,7 @@
       <c r="D14">
         <v>692</v>
       </c>
-      <c r="E14" s="9" t="str">
+      <c r="E14" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=13DegreePlanID=10TermID=4RequirementID=692</v>
       </c>
@@ -1418,7 +1437,7 @@
       <c r="D15">
         <v>460</v>
       </c>
-      <c r="E15" s="9" t="str">
+      <c r="E15" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=14DegreePlanID=11TermID=1RequirementID=460</v>
       </c>
@@ -1436,7 +1455,7 @@
       <c r="D16">
         <v>356</v>
       </c>
-      <c r="E16" s="9" t="str">
+      <c r="E16" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=15DegreePlanID=11TermID=1RequirementID=356</v>
       </c>
@@ -1454,7 +1473,7 @@
       <c r="D17">
         <v>542</v>
       </c>
-      <c r="E17" s="9" t="str">
+      <c r="E17" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=16DegreePlanID=11TermID=1RequirementID=542</v>
       </c>
@@ -1472,7 +1491,7 @@
       <c r="D18">
         <v>563</v>
       </c>
-      <c r="E18" s="9" t="str">
+      <c r="E18" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=17DegreePlanID=11TermID=1RequirementID=563</v>
       </c>
@@ -1490,7 +1509,7 @@
       <c r="D19">
         <v>560</v>
       </c>
-      <c r="E19" s="9" t="str">
+      <c r="E19" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=18DegreePlanID=11TermID=2RequirementID=560</v>
       </c>
@@ -1508,7 +1527,7 @@
       <c r="D20">
         <v>555</v>
       </c>
-      <c r="E20" s="9" t="str">
+      <c r="E20" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=19DegreePlanID=11TermID=2RequirementID=555</v>
       </c>
@@ -1526,7 +1545,7 @@
       <c r="D21">
         <v>618</v>
       </c>
-      <c r="E21" s="9" t="str">
+      <c r="E21" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=20DegreePlanID=11TermID=2RequirementID=618</v>
       </c>
@@ -1544,7 +1563,7 @@
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="E22" s="9" t="str">
+      <c r="E22" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=21DegreePlanID=11TermID=4RequirementID=1</v>
       </c>
@@ -1562,7 +1581,7 @@
       <c r="D23">
         <v>664</v>
       </c>
-      <c r="E23" s="9" t="str">
+      <c r="E23" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=22DegreePlanID=11TermID=4RequirementID=664</v>
       </c>
@@ -1580,7 +1599,7 @@
       <c r="D24">
         <v>691</v>
       </c>
-      <c r="E24" s="9" t="str">
+      <c r="E24" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=23DegreePlanID=11TermID=4RequirementID=691</v>
       </c>
@@ -1598,7 +1617,7 @@
       <c r="D25">
         <v>10</v>
       </c>
-      <c r="E25" s="9" t="str">
+      <c r="E25" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=24DegreePlanID=11TermID=5RequirementID=10</v>
       </c>
@@ -1616,7 +1635,7 @@
       <c r="D26">
         <v>20</v>
       </c>
-      <c r="E26" s="9" t="str">
+      <c r="E26" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=25DegreePlanID=11TermID=5RequirementID=20</v>
       </c>
@@ -1634,7 +1653,7 @@
       <c r="D27">
         <v>692</v>
       </c>
-      <c r="E27" s="9" t="str">
+      <c r="E27" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=26DegreePlanID=11TermID=5RequirementID=692</v>
       </c>
@@ -1652,7 +1671,7 @@
       <c r="D28" s="3">
         <v>460</v>
       </c>
-      <c r="E28" s="9" t="str">
+      <c r="E28" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=27DegreePlanID=30TermID=18RequirementID=460</v>
       </c>
@@ -1670,7 +1689,7 @@
       <c r="D29" s="3">
         <v>356</v>
       </c>
-      <c r="E29" s="9" t="str">
+      <c r="E29" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=28DegreePlanID=30TermID=18RequirementID=356</v>
       </c>
@@ -1688,7 +1707,7 @@
       <c r="D30" s="3">
         <v>542</v>
       </c>
-      <c r="E30" s="9" t="str">
+      <c r="E30" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=29DegreePlanID=30TermID=18RequirementID=542</v>
       </c>
@@ -1706,7 +1725,7 @@
       <c r="D31" s="3">
         <v>563</v>
       </c>
-      <c r="E31" s="9" t="str">
+      <c r="E31" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=30DegreePlanID=30TermID=18RequirementID=563</v>
       </c>
@@ -1724,7 +1743,7 @@
       <c r="D32" s="3">
         <v>560</v>
       </c>
-      <c r="E32" s="9" t="str">
+      <c r="E32" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=31DegreePlanID=30TermID=19RequirementID=560</v>
       </c>
@@ -1742,7 +1761,7 @@
       <c r="D33" s="3">
         <v>555</v>
       </c>
-      <c r="E33" s="9" t="str">
+      <c r="E33" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=32DegreePlanID=30TermID=19RequirementID=555</v>
       </c>
@@ -1760,7 +1779,7 @@
       <c r="D34" s="3">
         <v>618</v>
       </c>
-      <c r="E34" s="9" t="str">
+      <c r="E34" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=33DegreePlanID=30TermID=19RequirementID=618</v>
       </c>
@@ -1778,7 +1797,7 @@
       <c r="D35" s="3">
         <v>1</v>
       </c>
-      <c r="E35" s="9" t="str">
+      <c r="E35" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=34DegreePlanID=30TermID=21RequirementID=1</v>
       </c>
@@ -1796,7 +1815,7 @@
       <c r="D36" s="3">
         <v>664</v>
       </c>
-      <c r="E36" s="9" t="str">
+      <c r="E36" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=35DegreePlanID=30TermID=21RequirementID=664</v>
       </c>
@@ -1814,7 +1833,7 @@
       <c r="D37" s="3">
         <v>691</v>
       </c>
-      <c r="E37" s="9" t="str">
+      <c r="E37" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=36DegreePlanID=30TermID=21RequirementID=691</v>
       </c>
@@ -1832,7 +1851,7 @@
       <c r="D38" s="3">
         <v>10</v>
       </c>
-      <c r="E38" s="9" t="str">
+      <c r="E38" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=37DegreePlanID=30TermID=21RequirementID=10</v>
       </c>
@@ -1850,7 +1869,7 @@
       <c r="D39" s="3">
         <v>20</v>
       </c>
-      <c r="E39" s="9" t="str">
+      <c r="E39" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=38DegreePlanID=30TermID=22RequirementID=20</v>
       </c>
@@ -1868,7 +1887,7 @@
       <c r="D40" s="3">
         <v>692</v>
       </c>
-      <c r="E40" s="9" t="str">
+      <c r="E40" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=39DegreePlanID=30TermID=22RequirementID=692</v>
       </c>
@@ -1886,7 +1905,7 @@
       <c r="D41" s="3">
         <v>460</v>
       </c>
-      <c r="E41" s="9" t="str">
+      <c r="E41" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=40DegreePlanID=31TermID=18RequirementID=460</v>
       </c>
@@ -1904,7 +1923,7 @@
       <c r="D42" s="3">
         <v>356</v>
       </c>
-      <c r="E42" s="9" t="str">
+      <c r="E42" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=41DegreePlanID=31TermID=18RequirementID=356</v>
       </c>
@@ -1922,7 +1941,7 @@
       <c r="D43" s="3">
         <v>542</v>
       </c>
-      <c r="E43" s="9" t="str">
+      <c r="E43" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=42DegreePlanID=31TermID=18RequirementID=542</v>
       </c>
@@ -1940,7 +1959,7 @@
       <c r="D44" s="3">
         <v>563</v>
       </c>
-      <c r="E44" s="9" t="str">
+      <c r="E44" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=43DegreePlanID=31TermID=18RequirementID=563</v>
       </c>
@@ -1958,7 +1977,7 @@
       <c r="D45" s="3">
         <v>560</v>
       </c>
-      <c r="E45" s="9" t="str">
+      <c r="E45" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=44DegreePlanID=31TermID=19RequirementID=560</v>
       </c>
@@ -1976,7 +1995,7 @@
       <c r="D46" s="3">
         <v>555</v>
       </c>
-      <c r="E46" s="9" t="str">
+      <c r="E46" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=45DegreePlanID=31TermID=19RequirementID=555</v>
       </c>
@@ -1994,7 +2013,7 @@
       <c r="D47" s="3">
         <v>618</v>
       </c>
-      <c r="E47" s="9" t="str">
+      <c r="E47" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=46DegreePlanID=31TermID=19RequirementID=618</v>
       </c>
@@ -2012,7 +2031,7 @@
       <c r="D48" s="3">
         <v>1</v>
       </c>
-      <c r="E48" s="9" t="str">
+      <c r="E48" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=47DegreePlanID=31TermID=20RequirementID=1</v>
       </c>
@@ -2030,7 +2049,7 @@
       <c r="D49" s="3">
         <v>664</v>
       </c>
-      <c r="E49" s="9" t="str">
+      <c r="E49" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=48DegreePlanID=31TermID=21RequirementID=664</v>
       </c>
@@ -2048,7 +2067,7 @@
       <c r="D50" s="3">
         <v>691</v>
       </c>
-      <c r="E50" s="9" t="str">
+      <c r="E50" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=49DegreePlanID=31TermID=21RequirementID=691</v>
       </c>
@@ -2066,7 +2085,7 @@
       <c r="D51" s="3">
         <v>10</v>
       </c>
-      <c r="E51" s="9" t="str">
+      <c r="E51" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=50DegreePlanID=31TermID=21RequirementID=10</v>
       </c>
@@ -2084,7 +2103,7 @@
       <c r="D52" s="3">
         <v>20</v>
       </c>
-      <c r="E52" s="9" t="str">
+      <c r="E52" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=51DegreePlanID=31TermID=22RequirementID=20</v>
       </c>
@@ -2102,7 +2121,7 @@
       <c r="D53" s="3">
         <v>692</v>
       </c>
-      <c r="E53" s="9" t="str">
+      <c r="E53" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=52DegreePlanID=31TermID=22RequirementID=692</v>
       </c>
@@ -2120,7 +2139,7 @@
       <c r="D54" s="4">
         <v>542</v>
       </c>
-      <c r="E54" s="9" t="str">
+      <c r="E54" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=53DegreePlanID=12TermID=1RequirementID=542</v>
       </c>
@@ -2138,7 +2157,7 @@
       <c r="D55" s="4">
         <v>460</v>
       </c>
-      <c r="E55" s="9" t="str">
+      <c r="E55" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=54DegreePlanID=12TermID=1RequirementID=460</v>
       </c>
@@ -2156,7 +2175,7 @@
       <c r="D56" s="4">
         <v>356</v>
       </c>
-      <c r="E56" s="9" t="str">
+      <c r="E56" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=55DegreePlanID=12TermID=1RequirementID=356</v>
       </c>
@@ -2174,7 +2193,7 @@
       <c r="D57" s="4">
         <v>664</v>
       </c>
-      <c r="E57" s="9" t="str">
+      <c r="E57" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=56DegreePlanID=12TermID=3RequirementID=664</v>
       </c>
@@ -2192,7 +2211,7 @@
       <c r="D58" s="4">
         <v>1</v>
       </c>
-      <c r="E58" s="9" t="str">
+      <c r="E58" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=57DegreePlanID=12TermID=3RequirementID=1</v>
       </c>
@@ -2210,7 +2229,7 @@
       <c r="D59" s="4">
         <v>560</v>
       </c>
-      <c r="E59" s="9" t="str">
+      <c r="E59" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=58DegreePlanID=12TermID=3RequirementID=560</v>
       </c>
@@ -2228,7 +2247,7 @@
       <c r="D60" s="4">
         <v>691</v>
       </c>
-      <c r="E60" s="9" t="str">
+      <c r="E60" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=59DegreePlanID=12TermID=2RequirementID=691</v>
       </c>
@@ -2246,7 +2265,7 @@
       <c r="D61" s="4">
         <v>10</v>
       </c>
-      <c r="E61" s="9" t="str">
+      <c r="E61" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=60DegreePlanID=12TermID=2RequirementID=10</v>
       </c>
@@ -2264,7 +2283,7 @@
       <c r="D62" s="4">
         <v>692</v>
       </c>
-      <c r="E62" s="9" t="str">
+      <c r="E62" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=61DegreePlanID=12TermID=4RequirementID=692</v>
       </c>
@@ -2282,7 +2301,7 @@
       <c r="D63" s="4">
         <v>555</v>
       </c>
-      <c r="E63" s="9" t="str">
+      <c r="E63" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=62DegreePlanID=12TermID=4RequirementID=555</v>
       </c>
@@ -2300,7 +2319,7 @@
       <c r="D64" s="4">
         <v>563</v>
       </c>
-      <c r="E64" s="9" t="str">
+      <c r="E64" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=63DegreePlanID=12TermID=6RequirementID=563</v>
       </c>
@@ -2318,7 +2337,7 @@
       <c r="D65" s="4">
         <v>20</v>
       </c>
-      <c r="E65" s="9" t="str">
+      <c r="E65" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=64DegreePlanID=12TermID=6RequirementID=20</v>
       </c>
@@ -2336,7 +2355,7 @@
       <c r="D66" s="4">
         <v>618</v>
       </c>
-      <c r="E66" s="9" t="str">
+      <c r="E66" s="8" t="str">
         <f t="shared" si="0"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=65DegreePlanID=12TermID=6RequirementID=618</v>
       </c>
@@ -2354,7 +2373,7 @@
       <c r="D67" s="4">
         <v>356</v>
       </c>
-      <c r="E67" s="9" t="str">
+      <c r="E67" s="8" t="str">
         <f t="shared" ref="E67:E105" si="1">"new DegreePlanTermRequirement{"&amp;$A$1&amp;"="&amp;A67&amp;$B$1&amp;"="&amp;B67&amp;$C$1&amp;"="&amp;C67&amp;$D$1&amp;"="&amp;D67</f>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=66DegreePlanID=13TermID=1RequirementID=356</v>
       </c>
@@ -2372,7 +2391,7 @@
       <c r="D68" s="4">
         <v>460</v>
       </c>
-      <c r="E68" s="9" t="str">
+      <c r="E68" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=67DegreePlanID=13TermID=1RequirementID=460</v>
       </c>
@@ -2390,7 +2409,7 @@
       <c r="D69" s="4">
         <v>542</v>
       </c>
-      <c r="E69" s="9" t="str">
+      <c r="E69" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=68DegreePlanID=13TermID=1RequirementID=542</v>
       </c>
@@ -2408,7 +2427,7 @@
       <c r="D70" s="4">
         <v>563</v>
       </c>
-      <c r="E70" s="9" t="str">
+      <c r="E70" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=69DegreePlanID=13TermID=1RequirementID=563</v>
       </c>
@@ -2426,7 +2445,7 @@
       <c r="D71" s="4">
         <v>560</v>
       </c>
-      <c r="E71" s="9" t="str">
+      <c r="E71" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=70DegreePlanID=13TermID=3RequirementID=560</v>
       </c>
@@ -2444,7 +2463,7 @@
       <c r="D72" s="4">
         <v>1</v>
       </c>
-      <c r="E72" s="9" t="str">
+      <c r="E72" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=71DegreePlanID=13TermID=3RequirementID=1</v>
       </c>
@@ -2462,7 +2481,7 @@
       <c r="D73" s="4">
         <v>664</v>
       </c>
-      <c r="E73" s="9" t="str">
+      <c r="E73" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=72DegreePlanID=13TermID=3RequirementID=664</v>
       </c>
@@ -2480,7 +2499,7 @@
       <c r="D74" s="4">
         <v>10</v>
       </c>
-      <c r="E74" s="9" t="str">
+      <c r="E74" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=73DegreePlanID=13TermID=3RequirementID=10</v>
       </c>
@@ -2498,7 +2517,7 @@
       <c r="D75" s="4">
         <v>20</v>
       </c>
-      <c r="E75" s="9" t="str">
+      <c r="E75" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=74DegreePlanID=13TermID=4RequirementID=20</v>
       </c>
@@ -2516,7 +2535,7 @@
       <c r="D76" s="4">
         <v>691</v>
       </c>
-      <c r="E76" s="9" t="str">
+      <c r="E76" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=75DegreePlanID=13TermID=4RequirementID=691</v>
       </c>
@@ -2534,7 +2553,7 @@
       <c r="D77" s="4">
         <v>618</v>
       </c>
-      <c r="E77" s="9" t="str">
+      <c r="E77" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=76DegreePlanID=13TermID=4RequirementID=618</v>
       </c>
@@ -2552,7 +2571,7 @@
       <c r="D78" s="4">
         <v>692</v>
       </c>
-      <c r="E78" s="9" t="str">
+      <c r="E78" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=77DegreePlanID=13TermID=6RequirementID=692</v>
       </c>
@@ -2570,7 +2589,7 @@
       <c r="D79" s="4">
         <v>555</v>
       </c>
-      <c r="E79" s="9" t="str">
+      <c r="E79" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=78DegreePlanID=13TermID=6RequirementID=555</v>
       </c>
@@ -2588,7 +2607,7 @@
       <c r="D80" s="6">
         <v>460</v>
       </c>
-      <c r="E80" s="9" t="str">
+      <c r="E80" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=79DegreePlanID=14TermID=1RequirementID=460</v>
       </c>
@@ -2606,7 +2625,7 @@
       <c r="D81" s="6">
         <v>356</v>
       </c>
-      <c r="E81" s="9" t="str">
+      <c r="E81" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=80DegreePlanID=14TermID=1RequirementID=356</v>
       </c>
@@ -2624,7 +2643,7 @@
       <c r="D82" s="6">
         <v>542</v>
       </c>
-      <c r="E82" s="9" t="str">
+      <c r="E82" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=81DegreePlanID=14TermID=1RequirementID=542</v>
       </c>
@@ -2642,7 +2661,7 @@
       <c r="D83" s="6">
         <v>563</v>
       </c>
-      <c r="E83" s="9" t="str">
+      <c r="E83" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=82DegreePlanID=14TermID=1RequirementID=563</v>
       </c>
@@ -2660,7 +2679,7 @@
       <c r="D84" s="6">
         <v>560</v>
       </c>
-      <c r="E84" s="9" t="str">
+      <c r="E84" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=83DegreePlanID=14TermID=2RequirementID=560</v>
       </c>
@@ -2678,7 +2697,7 @@
       <c r="D85" s="6">
         <v>555</v>
       </c>
-      <c r="E85" s="9" t="str">
+      <c r="E85" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=84DegreePlanID=14TermID=2RequirementID=555</v>
       </c>
@@ -2696,7 +2715,7 @@
       <c r="D86" s="6">
         <v>664</v>
       </c>
-      <c r="E86" s="9" t="str">
+      <c r="E86" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=85DegreePlanID=14TermID=2RequirementID=664</v>
       </c>
@@ -2714,7 +2733,7 @@
       <c r="D87" s="6">
         <v>1</v>
       </c>
-      <c r="E87" s="9" t="str">
+      <c r="E87" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=86DegreePlanID=14TermID=4RequirementID=1</v>
       </c>
@@ -2732,7 +2751,7 @@
       <c r="D88" s="6">
         <v>618</v>
       </c>
-      <c r="E88" s="9" t="str">
+      <c r="E88" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=87DegreePlanID=14TermID=4RequirementID=618</v>
       </c>
@@ -2750,7 +2769,7 @@
       <c r="D89" s="6">
         <v>10</v>
       </c>
-      <c r="E89" s="9" t="str">
+      <c r="E89" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=88DegreePlanID=14TermID=4RequirementID=10</v>
       </c>
@@ -2768,7 +2787,7 @@
       <c r="D90" s="6">
         <v>691</v>
       </c>
-      <c r="E90" s="9" t="str">
+      <c r="E90" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=89DegreePlanID=14TermID=5RequirementID=691</v>
       </c>
@@ -2786,7 +2805,7 @@
       <c r="D91" s="6">
         <v>20</v>
       </c>
-      <c r="E91" s="9" t="str">
+      <c r="E91" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=90DegreePlanID=14TermID=5RequirementID=20</v>
       </c>
@@ -2804,7 +2823,7 @@
       <c r="D92" s="6">
         <v>692</v>
       </c>
-      <c r="E92" s="9" t="str">
+      <c r="E92" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=91DegreePlanID=14TermID=5RequirementID=692</v>
       </c>
@@ -2822,7 +2841,7 @@
       <c r="D93" s="6">
         <v>460</v>
       </c>
-      <c r="E93" s="9" t="str">
+      <c r="E93" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=92DegreePlanID=15TermID=1RequirementID=460</v>
       </c>
@@ -2840,7 +2859,7 @@
       <c r="D94" s="6">
         <v>356</v>
       </c>
-      <c r="E94" s="9" t="str">
+      <c r="E94" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=93DegreePlanID=15TermID=1RequirementID=356</v>
       </c>
@@ -2858,7 +2877,7 @@
       <c r="D95" s="6">
         <v>542</v>
       </c>
-      <c r="E95" s="9" t="str">
+      <c r="E95" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=94DegreePlanID=15TermID=1RequirementID=542</v>
       </c>
@@ -2876,7 +2895,7 @@
       <c r="D96" s="6">
         <v>563</v>
       </c>
-      <c r="E96" s="9" t="str">
+      <c r="E96" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=95DegreePlanID=15TermID=1RequirementID=563</v>
       </c>
@@ -2894,7 +2913,7 @@
       <c r="D97" s="6">
         <v>560</v>
       </c>
-      <c r="E97" s="9" t="str">
+      <c r="E97" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=96DegreePlanID=15TermID=2RequirementID=560</v>
       </c>
@@ -2912,7 +2931,7 @@
       <c r="D98" s="6">
         <v>664</v>
       </c>
-      <c r="E98" s="9" t="str">
+      <c r="E98" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=97DegreePlanID=15TermID=2RequirementID=664</v>
       </c>
@@ -2930,7 +2949,7 @@
       <c r="D99" s="6">
         <v>1</v>
       </c>
-      <c r="E99" s="9" t="str">
+      <c r="E99" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=98DegreePlanID=15TermID=2RequirementID=1</v>
       </c>
@@ -2948,7 +2967,7 @@
       <c r="D100" s="6">
         <v>555</v>
       </c>
-      <c r="E100" s="9" t="str">
+      <c r="E100" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=99DegreePlanID=15TermID=3RequirementID=555</v>
       </c>
@@ -2966,7 +2985,7 @@
       <c r="D101" s="6">
         <v>618</v>
       </c>
-      <c r="E101" s="9" t="str">
+      <c r="E101" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=100DegreePlanID=15TermID=3RequirementID=618</v>
       </c>
@@ -2984,7 +3003,7 @@
       <c r="D102" s="6">
         <v>691</v>
       </c>
-      <c r="E102" s="9" t="str">
+      <c r="E102" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=101DegreePlanID=15TermID=3RequirementID=691</v>
       </c>
@@ -3002,7 +3021,7 @@
       <c r="D103" s="6">
         <v>10</v>
       </c>
-      <c r="E103" s="9" t="str">
+      <c r="E103" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=102DegreePlanID=15TermID=4RequirementID=10</v>
       </c>
@@ -3020,7 +3039,7 @@
       <c r="D104" s="6">
         <v>20</v>
       </c>
-      <c r="E104" s="9" t="str">
+      <c r="E104" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=103DegreePlanID=15TermID=4RequirementID=20</v>
       </c>
@@ -3038,7 +3057,7 @@
       <c r="D105" s="6">
         <v>692</v>
       </c>
-      <c r="E105" s="9" t="str">
+      <c r="E105" s="8" t="str">
         <f t="shared" si="1"/>
         <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=104DegreePlanID=15TermID=4RequirementID=692</v>
       </c>
@@ -3050,16 +3069,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="3" width="24.42578125" customWidth="1"/>
     <col min="4" max="4" width="37.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="135.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3073,151 +3096,190 @@
         <v>29</v>
       </c>
       <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>10</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9">
+        <v>531367</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="5" t="str">
+        <f>"new DegreePlan{"&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;","&amp;$D$1&amp;"='"&amp;D2&amp;"',"&amp;$E$1&amp;"='"&amp;E2&amp;"'},"</f>
+        <v>new DegreePlan{DegreePlanID=10,DegreeID=1,StudentID=531367,DegreePlanAbrev='No summer off',DegreePlanName='No summer off'},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>11</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>531367</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="5" t="str">
+        <f t="shared" ref="F3:F9" si="0">"new DegreePlan{"&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;","&amp;$D$1&amp;"='"&amp;D3&amp;"',"&amp;$E$1&amp;"='"&amp;E3&amp;"'},"</f>
+        <v>new DegreePlan{DegreePlanID=11,DegreeID=1,StudentID=531367,DegreePlanAbrev='Summer Off',DegreePlanName='summer off'},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>30</v>
+      </c>
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+      <c r="C4" s="10">
+        <v>533900</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan{DegreePlanID=30,DegreeID=1,StudentID=533900,DegreePlanAbrev='No summer off',DegreePlanName='No summer off'},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>31</v>
+      </c>
+      <c r="B5" s="10">
+        <v>1</v>
+      </c>
+      <c r="C5" s="10">
+        <v>533900</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan{DegreePlanID=31,DegreeID=1,StudentID=533900,DegreePlanAbrev='Summer Off',DegreePlanName='summer off'},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>12</v>
+      </c>
+      <c r="B6" s="9">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9">
+        <v>533985</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan{DegreePlanID=12,DegreeID=1,StudentID=533985,DegreePlanAbrev='No summer off',DegreePlanName='No summer off'},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>13</v>
+      </c>
+      <c r="B7" s="9">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9">
+        <v>533985</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan{DegreePlanID=13,DegreeID=1,StudentID=533985,DegreePlanAbrev='Summer Off',DegreePlanName='summer off'},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>14</v>
+      </c>
+      <c r="B8" s="11">
+        <v>1</v>
+      </c>
+      <c r="C8" s="11">
+        <v>521315</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan{DegreePlanID=14,DegreeID=1,StudentID=521315,DegreePlanAbrev='No summer off',DegreePlanName='No summer off'},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>15</v>
+      </c>
+      <c r="B9" s="11">
+        <v>1</v>
+      </c>
+      <c r="C9" s="11">
+        <v>521315</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan{DegreePlanID=15,DegreeID=1,StudentID=521315,DegreePlanAbrev='Summer Off',DegreePlanName='summer off'},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>531367</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>531367</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>30</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3">
-        <v>533900</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>31</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>533900</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>533985</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>533985</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
-        <v>14</v>
-      </c>
-      <c r="B8" s="7">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7">
-        <v>521315</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>15</v>
-      </c>
-      <c r="B9" s="7">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7">
-        <v>521315</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3225,98 +3287,125 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="107.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
       <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>531367</v>
       </c>
       <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
         <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" t="s">
-        <v>47</v>
       </c>
       <c r="E2">
         <v>562438</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="str">
+        <f>"new Student{"&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$C$1&amp;"='"&amp;C2&amp;"',"&amp;$B$1&amp;"='"&amp;B2&amp;"',"&amp;$D$1&amp;"='"&amp;D2&amp;"',"&amp;$E$1&amp;"="&amp;E2&amp;"},"</f>
+        <v>new Student{StudentID=531367,LastName='Devineni',FirstName='Sai Sirisha',Snumber='s531367',_919number=562438},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>533985</v>
       </c>
       <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
         <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
       </c>
       <c r="E3">
         <v>569178</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F5" si="0">"new Student{"&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$C$1&amp;"='"&amp;C3&amp;"',"&amp;$B$1&amp;"='"&amp;B3&amp;"',"&amp;$D$1&amp;"='"&amp;D3&amp;"',"&amp;$E$1&amp;"="&amp;E3&amp;"},"</f>
+        <v>new Student{StudentID=533985,LastName='Marasini',FirstName='Dristi',Snumber='s533985',_919number=569178},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>521315</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>53</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="E4" s="6">
         <v>480684</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>new Student{StudentID=521315,LastName='Joshi',FirstName='Aawaj',Snumber='s521315',_919number=480684},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>533900</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="E5" s="3">
         <v>568896</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>new Student{StudentID=533900,LastName='Bourishetty',FirstName='Karun ',Snumber='s533900',_919number=568896},</v>
       </c>
     </row>
   </sheetData>
@@ -3325,7 +3414,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3342,16 +3431,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3365,7 +3454,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3379,7 +3468,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3393,7 +3482,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3407,7 +3496,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3421,7 +3510,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3435,7 +3524,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3449,7 +3538,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3463,7 +3552,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3477,7 +3566,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3491,7 +3580,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3505,7 +3594,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3519,7 +3608,7 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3533,7 +3622,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3547,7 +3636,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3561,7 +3650,7 @@
         <v>14</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3575,7 +3664,7 @@
         <v>15</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3589,7 +3678,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3603,7 +3692,7 @@
         <v>17</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3617,7 +3706,7 @@
         <v>18</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3631,7 +3720,7 @@
         <v>19</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3645,7 +3734,7 @@
         <v>20</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3659,7 +3748,7 @@
         <v>21</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Details with requirements in degree details
</commit_message>
<xml_diff>
--- a/Docs/DatabaseSamples.xlsx
+++ b/Docs/DatabaseSamples.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\masters\C#.net\MSACSDegreePlan\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531367\Documents\44663\MSACSDegreePlan\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90042941-AA92-4492-BB84-749DBE21EA17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
     <sheet name="Student" sheetId="6" r:id="rId6"/>
     <sheet name="StudentTerm" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="77">
   <si>
     <t>ACS+2</t>
   </si>
@@ -263,12 +264,15 @@
   </si>
   <si>
     <t>DegreePlanName</t>
+  </si>
+  <si>
+    <t>DegreeId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -637,10 +641,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -685,11 +689,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,7 +701,8 @@
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="6" max="6" width="79.140625" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="124.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -710,6 +715,9 @@
       <c r="C1" t="s">
         <v>68</v>
       </c>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -721,12 +729,15 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
       <c r="E2" t="s">
         <v>69</v>
       </c>
       <c r="F2" t="str">
-        <f>$E$2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;"'"&amp;B2&amp;"'"&amp;","&amp;$C$1&amp;"="&amp;"'"&amp;C2&amp;"'"&amp;$G$2</f>
-        <v>new Requirement{RequirementID=460,RequirementAbbrev='DB',RequirementName='44-460 Database'}</v>
+        <f>$E$2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;"'"&amp;B2&amp;"'"&amp;","&amp;$C$1&amp;"="&amp;"'"&amp;C2&amp;"'"&amp;","&amp;$D$1&amp;"="&amp;D2&amp;$G$2</f>
+        <v>new Requirement{RequirementID=460,RequirementAbbrev='DB',RequirementName='44-460 Database',DegreeId=1}</v>
       </c>
       <c r="G2" t="s">
         <v>66</v>
@@ -742,9 +753,12 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F14" si="0">$E$2&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;"'"&amp;B3&amp;"'"&amp;","&amp;$C$1&amp;"="&amp;"'"&amp;C3&amp;"'"&amp;$G$2</f>
-        <v>new Requirement{RequirementID=356,RequirementAbbrev='NF',RequirementName='44-356 Network Fundamemtals'}</v>
+        <f t="shared" ref="F3:F14" si="0">$E$2&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;"'"&amp;B3&amp;"'"&amp;","&amp;$C$1&amp;"="&amp;"'"&amp;C3&amp;"'"&amp;","&amp;$D$1&amp;"="&amp;D3&amp;$G$2</f>
+        <v>new Requirement{RequirementID=356,RequirementAbbrev='NF',RequirementName='44-356 Network Fundamemtals',DegreeId=1}</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -757,9 +771,12 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>new Requirement{RequirementID=542,RequirementAbbrev='OOP',RequirementName='44-542 OOP with Java'}</v>
+        <v>new Requirement{RequirementID=542,RequirementAbbrev='OOP',RequirementName='44-542 OOP with Java',DegreeId=1}</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -772,9 +789,12 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>new Requirement{RequirementID=563,RequirementAbbrev='Web apps',RequirementName='44-563 Web apps'}</v>
+        <v>new Requirement{RequirementID=563,RequirementAbbrev='Web apps',RequirementName='44-563 Web apps',DegreeId=1}</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -787,9 +807,12 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>new Requirement{RequirementID=560,RequirementAbbrev='ADB',RequirementName='44-560 ADB'}</v>
+        <v>new Requirement{RequirementID=560,RequirementAbbrev='ADB',RequirementName='44-560 ADB',DegreeId=1}</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -802,9 +825,12 @@
       <c r="C7" t="s">
         <v>15</v>
       </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>new Requirement{RequirementID=555,RequirementAbbrev='NS',RequirementName='44-555 Network Security'}</v>
+        <v>new Requirement{RequirementID=555,RequirementAbbrev='NS',RequirementName='44-555 Network Security',DegreeId=1}</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -817,9 +843,12 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>new Requirement{RequirementID=618,RequirementAbbrev='PM',RequirementName='44-618 PM'}</v>
+        <v>new Requirement{RequirementID=618,RequirementAbbrev='PM',RequirementName='44-618 PM',DegreeId=1}</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -832,9 +861,12 @@
       <c r="C9" t="s">
         <v>20</v>
       </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>new Requirement{RequirementID=1,RequirementAbbrev='Mobile',RequirementName='44-643 or 44-644'}</v>
+        <v>new Requirement{RequirementID=1,RequirementAbbrev='Mobile',RequirementName='44-643 or 44-644',DegreeId=1}</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -847,9 +879,12 @@
       <c r="C10" t="s">
         <v>22</v>
       </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>new Requirement{RequirementID=664,RequirementAbbrev='UX',RequirementName='44-664 UX'}</v>
+        <v>new Requirement{RequirementID=664,RequirementAbbrev='UX',RequirementName='44-664 UX',DegreeId=1}</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -862,9 +897,12 @@
       <c r="C11" t="s">
         <v>23</v>
       </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>new Requirement{RequirementID=10,RequirementAbbrev='E1',RequirementName='Elective 1'}</v>
+        <v>new Requirement{RequirementID=10,RequirementAbbrev='E1',RequirementName='Elective 1',DegreeId=1}</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -877,9 +915,12 @@
       <c r="C12" t="s">
         <v>24</v>
       </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>new Requirement{RequirementID=20,RequirementAbbrev='E2',RequirementName='Elective 2'}</v>
+        <v>new Requirement{RequirementID=20,RequirementAbbrev='E2',RequirementName='Elective 2',DegreeId=1}</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -892,9 +933,12 @@
       <c r="C13" t="s">
         <v>27</v>
       </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>new Requirement{RequirementID=691,RequirementAbbrev='GDP1',RequirementName='GDP1'}</v>
+        <v>new Requirement{RequirementID=691,RequirementAbbrev='GDP1',RequirementName='GDP1',DegreeId=1}</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -907,9 +951,12 @@
       <c r="C14" t="s">
         <v>28</v>
       </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>new Requirement{RequirementID=692,RequirementAbbrev='GDP2',RequirementName='GDP2'}</v>
+        <v>new Requirement{RequirementID=692,RequirementAbbrev='GDP2',RequirementName='GDP2',DegreeId=1}</v>
       </c>
     </row>
   </sheetData>
@@ -918,7 +965,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1158,7 +1205,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3069,7 +3116,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3287,7 +3334,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3414,7 +3461,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Drag and Drop implemented
</commit_message>
<xml_diff>
--- a/Docs/DatabaseSamples.xlsx
+++ b/Docs/DatabaseSamples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531367\Documents\44663\MSACSDegreePlan\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90042941-AA92-4492-BB84-749DBE21EA17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92E638A-C167-4CC2-AE85-C777EAA2A46C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="78">
   <si>
     <t>ACS+2</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>DegreeId</t>
+  </si>
+  <si>
+    <t>DegreePlanId</t>
   </si>
 </sst>
 </file>
@@ -341,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -360,6 +363,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -692,7 +698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F14"/>
     </sheetView>
   </sheetViews>
@@ -3119,8 +3125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3338,7 +3344,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3462,21 +3468,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="2" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -3484,181 +3490,220 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>531367</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="9">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>531367</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="9">
+        <v>10</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>531367</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="9">
+        <v>10</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>531367</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="9">
+        <v>10</v>
+      </c>
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>531367</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="9">
+        <v>10</v>
+      </c>
+      <c r="D6">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>531367</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="9">
+        <v>10</v>
+      </c>
+      <c r="D7">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>533985</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C8" s="12">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>533985</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="12">
+        <v>12</v>
+      </c>
+      <c r="D9">
         <v>2</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>533985</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="12">
+        <v>12</v>
+      </c>
+      <c r="D10">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>533985</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="12">
+        <v>12</v>
+      </c>
+      <c r="D11">
         <v>4</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>533985</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="12">
+        <v>12</v>
+      </c>
+      <c r="D12">
         <v>5</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>533985</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="12">
+        <v>12</v>
+      </c>
+      <c r="D13">
         <v>6</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -3666,13 +3711,16 @@
         <v>521315</v>
       </c>
       <c r="C14" s="6">
+        <v>14</v>
+      </c>
+      <c r="D14" s="6">
         <v>12</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -3680,13 +3728,16 @@
         <v>521315</v>
       </c>
       <c r="C15" s="6">
+        <v>14</v>
+      </c>
+      <c r="D15" s="6">
         <v>13</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -3696,11 +3747,14 @@
       <c r="C16" s="6">
         <v>14</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="6">
+        <v>14</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -3708,13 +3762,16 @@
         <v>521315</v>
       </c>
       <c r="C17" s="6">
+        <v>14</v>
+      </c>
+      <c r="D17" s="6">
         <v>15</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -3722,13 +3779,16 @@
         <v>521315</v>
       </c>
       <c r="C18" s="6">
+        <v>14</v>
+      </c>
+      <c r="D18" s="6">
         <v>16</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -3736,13 +3796,16 @@
         <v>533900</v>
       </c>
       <c r="C19" s="2">
+        <v>30</v>
+      </c>
+      <c r="D19" s="2">
         <v>17</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -3750,13 +3813,16 @@
         <v>533900</v>
       </c>
       <c r="C20" s="2">
+        <v>30</v>
+      </c>
+      <c r="D20" s="2">
         <v>18</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -3764,13 +3830,16 @@
         <v>533900</v>
       </c>
       <c r="C21" s="2">
+        <v>30</v>
+      </c>
+      <c r="D21" s="2">
         <v>19</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -3778,13 +3847,16 @@
         <v>533900</v>
       </c>
       <c r="C22" s="2">
+        <v>30</v>
+      </c>
+      <c r="D22" s="2">
         <v>20</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -3792,9 +3864,12 @@
         <v>533900</v>
       </c>
       <c r="C23" s="2">
+        <v>30</v>
+      </c>
+      <c r="D23" s="2">
         <v>21</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>